<commit_message>
add Reporter to the UFT Tests
</commit_message>
<xml_diff>
--- a/UFTOneAutomationTests/FlightLoginFailedAutomationTest/Default.xlsx
+++ b/UFTOneAutomationTests/FlightLoginFailedAutomationTest/Default.xlsx
@@ -4,12 +4,11 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
     <sheet name="1 Login" sheetId="2" r:id="rId2"/>
-    <sheet name="2 FailedToFindElement" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -474,12 +473,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.95"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -489,7 +488,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -502,23 +501,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.1"/>
-  <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="14.95" customFormat="1"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>